<commit_message>
Added graph to show all 6 trendlines
</commit_message>
<xml_diff>
--- a/BME 361/calibration_results.xlsx
+++ b/BME 361/calibration_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grace\source\repos\Uni-Projects\BME 361\Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Uni-Projects\BME 361\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C26510-6BE9-4AA2-9BE9-6A048C161B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB4A86E-1DEF-4541-AB3B-FBF023E06DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -1949,6 +1949,1276 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-HK"/>
+              <a:t>Calibration Trendlines</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13050643566073147"/>
+          <c:y val="0.1509190644641116"/>
+          <c:w val="0.82210876488239015"/>
+          <c:h val="0.72028279202335799"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>r0_1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10229</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10229</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.7799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.74</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.53</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-8C68-4492-9B3B-280D2397CE82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>r2_1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10229</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2556.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.03</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.88</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.38</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-8C68-4492-9B3B-280D2397CE82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>r6_1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$D$2:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10229</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10229</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>425.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.069999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.39</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.56</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-8C68-4492-9B3B-280D2397CE82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>r0_2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="lgDashDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$F$2:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.58</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.51</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8C68-4492-9B3B-280D2397CE82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>r2_2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="lgDashDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$G$2:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>929</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>486.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.58</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8C68-4492-9B3B-280D2397CE82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>r6_2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="lgDashDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$H$2:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49.15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.61</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8C68-4492-9B3B-280D2397CE82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="962779456"/>
+        <c:axId val="962781536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="962779456"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1300"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Mass (g)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.50366108233777418"/>
+              <c:y val="0.9086295717333569"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="962781536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="962781536"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="50000"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Resistance (k</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Ω</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.1195983852480404E-2"/>
+              <c:y val="0.32261499960111029"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="962779456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2069,6 +3339,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3102,6 +4412,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3722,6 +5548,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D53C2031-DF01-4A50-9572-7FCC4FADFA85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4029,8 +5893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>